<commit_message>
code REFACTORED using arraylist to writing data to excel
</commit_message>
<xml_diff>
--- a/src/main/resources/ExcelFiles/employee.xlsx
+++ b/src/main/resources/ExcelFiles/employee.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>EmpID</t>
   </si>
@@ -36,6 +36,9 @@
   </si>
   <si>
     <t>Scott</t>
+  </si>
+  <si>
+    <t>Data Analyst</t>
   </si>
 </sst>
 </file>
@@ -127,7 +130,7 @@
         <v>7</v>
       </c>
       <c r="C4" t="s">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>